<commit_message>
Backup QR Scanner data - 2025-12-11T06:51:22.900Z - Cache Bust: 1765435882900
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Pharmacology_scanner1765434733049_8d2713030f9c3056a2c8fb05645d0b171b0edafe9c611d2d79fb8421c37aab47.xlsx
+++ b/log_history/Y2_B2526_Pharmacology_scanner1765434733049_8d2713030f9c3056a2c8fb05645d0b171b0edafe9c611d2d79fb8421c37aab47.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Pharmacology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -802,9 +802,49 @@
         <v>nancy.abdelshafy@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>244939</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Pharmacology</v>
+      </c>
+      <c r="C21" t="str">
+        <v>11/12/2025</v>
+      </c>
+      <c r="D21" t="str">
+        <v>08:46:09</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F21" t="str">
+        <v>nancy.abdelshafy@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>244826</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Pharmacology</v>
+      </c>
+      <c r="C22" t="str">
+        <v>11/12/2025</v>
+      </c>
+      <c r="D22" t="str">
+        <v>08:51:07</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F22" t="str">
+        <v>nancy.abdelshafy@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>